<commit_message>
Mockups y lista de servicios de configuración de bicicletas actualizado
</commit_message>
<xml_diff>
--- a/docs/Servicios - interfaces/domicilios_reportes_mibici.xlsx
+++ b/docs/Servicios - interfaces/domicilios_reportes_mibici.xlsx
@@ -9,14 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Domicilios" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="4" r:id="rId2"/>
-    <sheet name="Reportes" sheetId="2" r:id="rId3"/>
-    <sheet name="Hoja2" sheetId="5" r:id="rId4"/>
-    <sheet name="miBici" sheetId="3" r:id="rId5"/>
+    <sheet name="Reportes" sheetId="4" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="5" r:id="rId3"/>
+    <sheet name="miBici" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162912"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="192">
   <si>
     <t>Nombre</t>
   </si>
@@ -736,226 +735,6 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">{
-      "user": "toro",
-      "start": "2015-09-23 10:00",
-      "finish": "2015-09-24 14:00"
-}
-</t>
-  </si>
-  <si>
-    <t>Mensaje OK:
-{
-    "code": 0,
-    "value": "info",
-    "description": "Finalizó Correctamente"    
-      "data": [
-           {
-               "nombre": "casa-trabajo",
-               "pInicio": "41.40338, 2.17403",
-               "pFin": "41.40338, 2.17403",
-               "fechaHora": "2015-09-24 07:30"
-                  "puntos": [
-                       "punto": "41.40338, 2.17403",
-                       "punto": "41.40338, 2.17403"                             ] 
-          {
-           },
-           {
-               "nombre": "casa-colegio",
-               "pInicio": "41.40338, 2.17403",
-               "pFin": "41.40338, 2.17403",
-               "fechaHora": "2015-09-24 07:30"
-                  "puntos": [
-                       "punto": "41.40338, 2.17403",
-                       "punto": "41.40338, 2.17403"                             ]        
-           },
-    ]
-}</t>
-  </si>
-  <si>
-    <t>Se retorna la información de los puntos almacenados para dicha ruta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-{
-      "user": "toro",
-      "start": "2015-09-23 10:00",
-      "finish": "2015-09-24 14:00"
-}
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mensaje OK:
-{
-    "code": 0,
-    "value": "info",
-    "description": "Finalizó Correctamente"    
-      "data": [
-            {
-               "day": "total",
-               "time": 1650 seg,
-               "distance": 35000 m,
-           },
-            {
-               "day": "2015-09-24",
-               "time": 165 seg,
-               "distance": 50 m,
-           },
-    ]
-}
-</t>
-  </si>
-  <si>
-    <t>exportarReporteRutas</t>
-  </si>
-  <si>
-    <t>Como usuario quiero obtener un archivo con el reporte de las rutas frecuentes</t>
-  </si>
-  <si>
-    <t>usuario 
-fecha inicio 
-fecha fin
-tipo archivo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-{
-      "user": "toro",
-      "start": "2015-09-23 10:00",
-      "finish": "2015-09-24 14:00"
-      "type": "1"
-}
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mensaje OK:
-{
-    "code": 0,
-    "value": "info",
-    "description": "Finalizó Correctamente"    
-      "data": [
-            {
-               "file": "C:/reportes/reporte_20150912.pdf",
-           },
-    ]
-}
-</t>
-  </si>
-  <si>
-    <t>Mensaje Entrada:
-Posibles valores para el campo type:
-1:PDF
-2:Excel
-3:JPG
-4:WORD</t>
-  </si>
-  <si>
-    <t>exportarReportetiempoDistancia</t>
-  </si>
-  <si>
-    <t>Como usuario quiero obtener un archivo con el reporte de tiempo y distancia recorridos</t>
-  </si>
-  <si>
-    <t>consultarNotificaciones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-{
-      "user": "toro",
-      "start": "2015-09-23 10:00",
-      "finish": "2015-09-24 14:00"
-      "type": "0"
-}
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mensaje OK:
-{
-    "code": 0,
-    "value": "info",
-    "description": "Finalizó Correctamente"    
-      "data": [
-            {
-               "type": "0",
-               "count": 50,
-           },
-           {
-               "type": "3",
-               "count": 50,
-           },
-    ]
-}
-</t>
-  </si>
-  <si>
-    <t>Mensaje Entrada:
-Posibles valores para el campo type:
-0: Todas
-1:SMS
-2:email
-3:llamada
-Si el parametro type es 0 entonces se devolvera la informacion total y la detallada</t>
-  </si>
-  <si>
-    <t>{
-   "idServicio": 76498764
-}</t>
-  </si>
-  <si>
-    <t>{
-    "usuario": "lbadillo"
-}</t>
-  </si>
-  <si>
-    <t>Mensaje OK:
-{
-    "codigo": 0,
-    "valor": "INFO",
-    "descripcion": "OK",
-    "datos": [
-        {
-            "nombre": "Ludwing",
-            "apellido": "Badillo",
-            "mail": "l.badillo10@uniandes.edu.co",
-            "celular": "3104567890",
-            "puntuacion": [
-                {
-                    "idServicio": 547657,
-                    "puntos": 8,
-                    "comentarios": "Buen trabajo"
-                },
-                {
-                    "idServicio": 55547657,
-                    "puntos": 3,
-                    "comentarios": "Mal  trabajo"
-                }
-            ]
-        }
-    ]
-}
-Mensaje Fallo:
-{
-    "codigo": 101,
-    "valor": "ERROR",
-    "descripcion": "Descripción error"
-}</t>
-  </si>
-  <si>
-    <t>{
-    "usuario": "lbadillo",
-    "idServicio": 969876,
-    "real": "00:20"
-}</t>
-  </si>
-  <si>
-    <t>{
-    "usuario": "lbadillo",
-    "idServicio": 969876,
-    "puntos": 9,
-    "comentarios": "buen trabajo"
-}</t>
-  </si>
-  <si>
     <t>Domicilios</t>
   </si>
   <si>
@@ -1137,24 +916,24 @@
   </si>
   <si>
     <t>{
-  "user": "toro",
-  "consulta": "1",
-  "config": [
-    {
-      "marco": "1",
-      "tijera": "4",
-      "ruedas": "6",
-      "frenos": "9",
-      "manubrio": "1",
-      "sillin": "2",
-      "tuboSillin": "8",
-      "cambios": "6",
-      "platoDelantero": "140",
-      "platoTrasero": "12",
-      "pedales": "3",
-      "cadena": "1"
-    }
-  ]
+  "user": "toro",
+  "consulta": "1",
+  "config": [
+    {
+      "marco": "1",
+      "tijera": "4",
+      "ruedas": "6",
+      "frenos": "9",
+      "manubrio": "1",
+      "sillin": "2",
+      "tuboSillin": "8",
+      "cambios": "6",
+      "platoDelantero": "140",
+      "platoTrasero": "12",
+      "pedales": "3",
+      "cadena": "1"
+    }
+  ]
 }</t>
   </si>
   <si>
@@ -1183,6 +962,49 @@
 1- Es una consulta de la configuracion</t>
   </si>
   <si>
+    <t>verOrden</t>
+  </si>
+  <si>
+    <t>Como usuario del sistema deseo ver las ordenes que he realizado</t>
+  </si>
+  <si>
+    <t>usuario
+idOrden</t>
+  </si>
+  <si>
+    <t>{
+  "user": "toro",
+  "consulta": "1",
+  "config": {
+    "usuario": "toroj",
+    "idOrden": "4098"
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  "codigo": 0,
+  "valor": "INFO",
+  "descripcion": "OK",
+  "datos": [
+    {
+      "marco": "1",
+      "tijera": "4",
+      "ruedas": "6",
+      "frenos": "9",
+      "manubrio": "1",
+      "sillin": "2",
+      "tuboSillin": "8",
+      "cambios": "6",
+      "platoDelantero": "140",
+      "platoTrasero": "12",
+      "pedales": "3",
+      "cadena": "1"
+    }
+  ]
+}</t>
+  </si>
+  <si>
     <t>Como usuario quiero consultar los tipos de productos disponibles para una parte especifica</t>
   </si>
   <si>
@@ -1192,31 +1014,35 @@
   <si>
     <t>{
    "usuario": "toro",
-   "tipoParte": "1"
-}</t>
-  </si>
-  <si>
-    <t>Mensaje OK:
-{
+   "tipoParte": "marco"
+}</t>
+  </si>
+  <si>
+    <t>{
   "codigo": 0,
-  "valor": "info",
-  "descripcion": "Finalizó Correctamente",
+  "valor": "INFO",
+  "descripcion": "OK",
   "datos": [
     {
-      "id": 2,
-      "nombre": "nombreProd",
-      "descripcion": "caracteristicas",
-      "disponible": "SI",
-      "imagen": "http://",
-      "precio": "150.000"
+      "idParte": 3,
+      "nombre": "marco el gato",
+      "descripcion": "",
+      "valor": "190.000",
+      "imagen": null
     },
     {
-      "id": 5,
-      "nombre": "nombre-prod",
-      "descriptcon": "caracteristicas",
-      "disponible": "NO",
-      "imagen": "http://",
-      "precio": "150.000"
+      "idParte": 4,
+      "nombre": "marco el perro",
+      "descripcion": "",
+      "valor": "10.000",
+      "imagen": null
+    },
+    {
+      "idParte": 5,
+      "nombre": "marco el tete",
+      "descripcion": "",
+      "valor": "10.000",
+      "imagen": null
     }
   ]
 }</t>
@@ -1229,7 +1055,6 @@
 4: frenos
 5: manubrio
 6: sillin
-7: tuboSillin
 8: cambios
 9: platoDelantero
 10: platoTrasero
@@ -1562,9 +1387,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1679,6 +1501,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1985,281 +1810,281 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="3"/>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="236.25">
-      <c r="A2" s="12">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="15" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="236.25">
-      <c r="A3" s="12">
+      <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="191.25">
-      <c r="A4" s="19">
+      <c r="A4" s="18">
         <v>3</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="21" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="135">
-      <c r="A5" s="12">
+      <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="17"/>
-      <c r="I5" s="16" t="s">
+      <c r="H5" s="16"/>
+      <c r="I5" s="15" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="135">
-      <c r="A6" s="12">
+      <c r="A6" s="11">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="17" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="135">
-      <c r="A7" s="12">
+      <c r="A7" s="11">
         <v>6</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="18" t="s">
+      <c r="H7" s="16"/>
+      <c r="I7" s="17" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="371.25">
-      <c r="A8" s="23">
+      <c r="A8" s="22">
         <v>7</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="26" t="s">
+      <c r="G8" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="27" t="s">
+      <c r="I8" s="26" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="135">
-      <c r="A9" s="12">
+      <c r="A9" s="11">
         <v>8</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="18" t="s">
+      <c r="H9" s="16"/>
+      <c r="I9" s="17" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="165.75">
-      <c r="A10" s="12">
+      <c r="A10" s="11">
         <v>9</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12" t="s">
+      <c r="H10" s="11"/>
+      <c r="I10" s="11" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2280,252 +2105,252 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" style="31" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" style="30" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="31" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" style="30" customWidth="1"/>
-    <col min="7" max="7" width="78.85546875" style="30" customWidth="1"/>
-    <col min="8" max="8" width="41.7109375" style="31" customWidth="1"/>
-    <col min="9" max="9" width="28.42578125" style="31" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="30" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="29" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="30" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" style="29" customWidth="1"/>
+    <col min="7" max="7" width="78.85546875" style="29" customWidth="1"/>
+    <col min="8" max="8" width="41.7109375" style="30" customWidth="1"/>
+    <col min="9" max="9" width="28.42578125" style="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="30" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="342.75" customHeight="1">
-      <c r="A2" s="29">
+      <c r="A2" s="28">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="I2" s="47" t="s">
+      <c r="I2" s="46" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="342.75" customHeight="1">
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="I3" s="47" t="s">
+      <c r="I3" s="46" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="342.75" customHeight="1">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="I4" s="47" t="s">
+      <c r="I4" s="46" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="306">
-      <c r="A5" s="42">
+      <c r="A5" s="41">
         <v>2</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="D5" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="44" t="s">
+      <c r="E5" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="44" t="s">
+      <c r="F5" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="G5" s="44" t="s">
+      <c r="G5" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
     </row>
     <row r="6" spans="1:9" ht="140.25">
-      <c r="A6" s="29">
+      <c r="A6" s="28">
         <v>3</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="31" t="s">
+      <c r="G6" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="31" t="s">
+      <c r="H6" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="I6" s="47" t="s">
+      <c r="I6" s="46" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="46" customFormat="1" ht="204">
-      <c r="A7" s="42">
+    <row r="7" spans="1:9" s="45" customFormat="1" ht="204">
+      <c r="A7" s="41">
         <v>4</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="E7" s="44" t="s">
+      <c r="E7" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="44" t="s">
+      <c r="F7" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="G7" s="44" t="s">
+      <c r="G7" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="H7" s="45" t="s">
+      <c r="H7" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="I7" s="44"/>
+      <c r="I7" s="43"/>
     </row>
     <row r="8" spans="1:9" ht="139.5" customHeight="1">
-      <c r="A8" s="29">
+      <c r="A8" s="28">
         <v>5</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="G8" s="31"/>
-      <c r="H8" s="41" t="s">
+      <c r="G8" s="30"/>
+      <c r="H8" s="40" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="139.5" customHeight="1">
-      <c r="A9" s="29">
+      <c r="A9" s="28">
         <v>6</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="H9" s="41"/>
+      <c r="H9" s="40"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2540,291 +2365,6 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
-  <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
-    <col min="7" max="7" width="41.7109375" customWidth="1"/>
-    <col min="8" max="8" width="35.5703125" customWidth="1"/>
-    <col min="9" max="9" width="26" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
-      <c r="A1" s="3"/>
-      <c r="B1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="303.75">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="I2" s="16"/>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" ht="213.75">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="16"/>
-    </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" ht="135">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="I4" s="22"/>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="135">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="I5" s="16"/>
-    </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" ht="191.25">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="I6" s="18"/>
-    </row>
-    <row r="7" spans="1:9" ht="135">
-      <c r="A7" s="12">
-        <v>6</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="18"/>
-    </row>
-    <row r="8" spans="1:9" ht="360.75">
-      <c r="A8" s="23">
-        <v>7</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="25" t="s">
-        <v>122</v>
-      </c>
-      <c r="G8" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="H8" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="27"/>
-    </row>
-    <row r="9" spans="1:9" ht="135">
-      <c r="A9" s="12">
-        <v>8</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="18"/>
-    </row>
-    <row r="10" spans="1:9" ht="153">
-      <c r="A10" s="12">
-        <v>9</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2833,291 +2373,291 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" style="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" style="34" customWidth="1"/>
-    <col min="3" max="3" width="25" style="34" customWidth="1"/>
-    <col min="4" max="4" width="31" style="34" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" style="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="33" customWidth="1"/>
+    <col min="3" max="3" width="25" style="33" customWidth="1"/>
+    <col min="4" max="4" width="31" style="33" customWidth="1"/>
     <col min="5" max="5" width="29.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="27.7109375" customWidth="1"/>
     <col min="7" max="10" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22.5" customHeight="1">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="39"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="34"/>
+      <c r="C6" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="34"/>
+      <c r="C7" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="34"/>
+      <c r="C8" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="39" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="D11" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="36" t="s">
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="B12" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="C12" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="D12" s="39" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="39" t="s">
+    <row r="13" spans="1:7">
+      <c r="A13" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="B13" s="39" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="39" t="s">
+      <c r="C13" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D13" s="39" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="39" t="s">
+    <row r="14" spans="1:7">
+      <c r="A14" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="B14" s="39" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="C5" s="39" t="s">
+      <c r="C14" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="D5" s="40"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="39" t="s">
+      <c r="D14" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="D6" s="40" t="s">
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="39" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="39" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="39" t="s">
+      <c r="B15" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="C15" s="39" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="39" t="s">
+      <c r="D15" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="D8" s="40" t="s">
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="34"/>
+      <c r="B16" s="39" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="40" t="s">
+      <c r="C16" s="39" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="37" t="s">
+      <c r="D16" s="39"/>
+    </row>
+    <row r="17" spans="1:4" ht="24">
+      <c r="A17" s="34"/>
+      <c r="B17" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="C17" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="D17" s="34"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="34"/>
+      <c r="B18" s="39" t="s">
         <v>147</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="C18" s="39" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="40" t="s">
+      <c r="D18" s="34"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="34"/>
+      <c r="B19" s="39" t="s">
         <v>149</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="C19" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="D19" s="34"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="34"/>
+      <c r="B20" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="C20" s="39" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="40" t="s">
+      <c r="D20" s="34"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="34"/>
+      <c r="B21" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="C21" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="D21" s="34"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="34"/>
+      <c r="B22" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="C22" s="39" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="40" t="s">
-        <v>157</v>
-      </c>
-      <c r="B14" s="40" t="s">
-        <v>158</v>
-      </c>
-      <c r="C14" s="40" t="s">
-        <v>159</v>
-      </c>
-      <c r="D14" s="40" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="40" t="s">
-        <v>161</v>
-      </c>
-      <c r="B15" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="C15" s="40" t="s">
-        <v>163</v>
-      </c>
-      <c r="D15" s="40" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="35"/>
-      <c r="B16" s="40" t="s">
-        <v>165</v>
-      </c>
-      <c r="C16" s="40" t="s">
-        <v>166</v>
-      </c>
-      <c r="D16" s="40"/>
-    </row>
-    <row r="17" spans="1:4" ht="24">
-      <c r="A17" s="35"/>
-      <c r="B17" s="40" t="s">
-        <v>167</v>
-      </c>
-      <c r="C17" s="40" t="s">
-        <v>168</v>
-      </c>
-      <c r="D17" s="35"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="35"/>
-      <c r="B18" s="40" t="s">
-        <v>169</v>
-      </c>
-      <c r="C18" s="40" t="s">
-        <v>170</v>
-      </c>
-      <c r="D18" s="35"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="35"/>
-      <c r="B19" s="40" t="s">
-        <v>171</v>
-      </c>
-      <c r="C19" s="40" t="s">
-        <v>172</v>
-      </c>
-      <c r="D19" s="35"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="35"/>
-      <c r="B20" s="40" t="s">
-        <v>173</v>
-      </c>
-      <c r="C20" s="40" t="s">
-        <v>174</v>
-      </c>
-      <c r="D20" s="35"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="35"/>
-      <c r="B21" s="40" t="s">
-        <v>175</v>
-      </c>
-      <c r="C21" s="40" t="s">
-        <v>176</v>
-      </c>
-      <c r="D21" s="35"/>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="35"/>
-      <c r="B22" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="C22" s="40" t="s">
-        <v>178</v>
-      </c>
-      <c r="D22" s="35"/>
+      <c r="D22" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -3127,7 +2667,7 @@
     <col min="3" max="3" width="25.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" style="47" customWidth="1"/>
     <col min="7" max="7" width="37.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="45.5703125" style="2" customWidth="1"/>
     <col min="9" max="16384" width="11.42578125" style="1"/>
@@ -3135,25 +2675,25 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3"/>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3162,177 +2702,201 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>182</v>
+        <v>159</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>160</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="270">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="236.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="225">
+      <c r="F3" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" ht="315">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>189</v>
+        <v>111</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>167</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>190</v>
+        <v>168</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" ht="135">
+        <v>11</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="225">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>193</v>
+        <v>113</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>172</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="1:8" ht="165.75">
+        <v>24</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="135">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="168.75">
+      <c r="F6" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" ht="165.75">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="202.5">
+      <c r="F7" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="168.75">
       <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>200</v>
+      <c r="F8" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="202.5">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Módulo Configuración conectado con los servicios
</commit_message>
<xml_diff>
--- a/docs/Servicios - interfaces/domicilios_reportes_mibici.xlsx
+++ b/docs/Servicios - interfaces/domicilios_reportes_mibici.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="204">
   <si>
     <t>Nombre</t>
   </si>
@@ -895,6 +895,9 @@
     <t>getConexion</t>
   </si>
   <si>
+    <t>ENDPOINT</t>
+  </si>
+  <si>
     <t>Como usuario de bicicleta configuro un producto y lo solicito</t>
   </si>
   <si>
@@ -906,7 +909,6 @@
 frenos
 manubrio
 sillin
-tuboSillin
 cambios
 platoDelantero
 platoTrasero
@@ -916,22 +918,21 @@
   </si>
   <si>
     <t>{
-  "user": "toro",
-  "consulta": "1",
+  "usuario": "toroj",
+  "consulta": "0",
   "config": [
     {
       "marco": "1",
       "tijera": "4",
-      "ruedas": "6",
-      "frenos": "9",
-      "manubrio": "1",
-      "sillin": "2",
-      "tuboSillin": "8",
-      "cambios": "6",
-      "platoDelantero": "140",
-      "platoTrasero": "12",
-      "pedales": "3",
-      "cadena": "1"
+      "ruedas": "0",
+      "frenos": "0",
+      "manubrio": "0",
+      "sillin": "0",
+      "cambios": "0",
+      "platoDelantero": "0",
+      "platoTrasero": "0",
+      "pedales": "0",
+      "cadena": "0"
     }
   ]
 }</t>
@@ -939,14 +940,14 @@
   <si>
     <t>Mensaje OK:
 {
-  "codigo": 0,
-  "valor": "info",
-  "descripcion": "Finalizó Correctamente",
-  "datos": 
-    {
-      "idOrden": 123,
-      "precio": "1,500,000"
-    }
+  "codigo": 0,
+  "valor": "info",
+  "descripcion": "Finalizó Correctamente",
+  "datos": 
+    {
+      "idOrden": "123000",
+      "precio": "1500000"
+    }
 }
 Mensaje Fallo:
 {
@@ -962,6 +963,9 @@
 1- Es una consulta de la configuracion</t>
   </si>
   <si>
+    <t>http://localhost:8080/bicitoolsMi/serviciosRest/miBici/verificarConfiguracion</t>
+  </si>
+  <si>
     <t>verOrden</t>
   </si>
   <si>
@@ -973,12 +977,11 @@
   </si>
   <si>
     <t>{
-  "user": "toro",
-  "consulta": "1",
-  "config": {
-    "usuario": "toroj",
-    "idOrden": "4098"
-  }
+  "user": "toroj",
+  "config": {
+    "usuario": "toroj",
+    "idOrden": "4098"
+  }
 }</t>
   </si>
   <si>
@@ -988,21 +991,95 @@
   "descripcion": "OK",
   "datos": [
     {
-      "marco": "1",
-      "tijera": "4",
-      "ruedas": "6",
-      "frenos": "9",
-      "manubrio": "1",
-      "sillin": "2",
-      "tuboSillin": "8",
-      "cambios": "6",
-      "platoDelantero": "140",
-      "platoTrasero": "12",
-      "pedales": "3",
-      "cadena": "1"
+      "idOrden": "659868",
+      "valor": "645210",
+      "fechaHora": "11/07/2015 16:39:08",
+      "estado": "Pendiente",
+      "partes": [
+        {
+          "idParte": "1",
+          "tipoParte": null,
+          "nombre": "pedales pato",
+          "valor": "115.210",
+          "descripcion": ""
+        },
+        {
+          "idParte": "4",
+          "tipoParte": "cadena",
+          "nombre": "cadena generica",
+          "valor": "100000",
+          "descripcion": null
+        },
+        {
+          "idParte": "8",
+          "tipoParte": "ruedas",
+          "nombre": "ruedas genericas",
+          "valor": "30000",
+          "descripcion": null
+        },
+        {
+          "idParte": "9",
+          "tipoParte": "frenos",
+          "nombre": "frenos genericos",
+          "valor": "40000",
+          "descripcion": null
+        },
+        {
+          "idParte": "10",
+          "tipoParte": "manubrio",
+          "nombre": "manubrio generico",
+          "valor": "50000",
+          "descripcion": null
+        },
+        {
+          "idParte": "11",
+          "tipoParte": "sillin",
+          "nombre": "sillin generico",
+          "valor": "60000",
+          "descripcion": null
+        },
+        {
+          "idParte": "12",
+          "tipoParte": "cambios",
+          "nombre": "cambios genericos",
+          "valor": "0",
+          "descripcion": "por defecto una bicicleta no tiene cambios"
+        },
+        {
+          "idParte": "13",
+          "tipoParte": "platodelantero",
+          "nombre": "plato delantero generico",
+          "valor": "70000",
+          "descripcion": null
+        },
+        {
+          "idParte": "14",
+          "tipoParte": "platotrasero",
+          "nombre": "plato trasero generico",
+          "valor": "80000",
+          "descripcion": null
+        },
+        {
+          "idParte": "15",
+          "tipoParte": "pedales",
+          "nombre": "pedales genericos",
+          "valor": "90000",
+          "descripcion": null
+        },
+        {
+          "idParte": "16",
+          "tipoParte": "cadena",
+          "nombre": "cadena generica",
+          "valor": "100000",
+          "descripcion": null
+        }
+      ]
     }
   ]
 }</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/bicitoolsMi/serviciosRest/miBici/detalleOrden</t>
   </si>
   <si>
     <t>Como usuario quiero consultar los tipos de productos disponibles para una parte especifica</t>
@@ -1024,24 +1101,24 @@
   "descripcion": "OK",
   "datos": [
     {
-      "idParte": 3,
+      "idParte": "3",
       "nombre": "marco el gato",
       "descripcion": "",
       "valor": "190.000",
       "imagen": null
     },
     {
-      "idParte": 4,
-      "nombre": "marco el perro",
+      "idParte": "5",
+      "nombre": "marco el tete",
       "descripcion": "",
       "valor": "10.000",
       "imagen": null
     },
     {
-      "idParte": 5,
-      "nombre": "marco el tete",
+      "idParte": "6",
+      "nombre": "marco el pelado",
       "descripcion": "",
-      "valor": "10.000",
+      "valor": "20.000",
       "imagen": null
     }
   ]
@@ -1055,11 +1132,14 @@
 4: frenos
 5: manubrio
 6: sillin
-8: cambios
-9: platoDelantero
-10: platoTrasero
-11: pedales
-12: cadena</t>
+7: cambios
+8: platoDelantero
+9: platoTrasero
+10: pedales
+11: cadena</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/bicitoolsMi/serviciosRest/miBici/consultarPartexTipo</t>
   </si>
   <si>
     <t>Como usuario de la aplicación quiero consultar los proveedores de un producto en particular</t>
@@ -1128,6 +1208,9 @@
 }</t>
   </si>
   <si>
+    <t>http://localhost:8080/bicitoolsMi/serviciosRest/miBici/insertarProveedor</t>
+  </si>
+  <si>
     <t>Yo como proveedor de bicicletas quiero agregar un producto a mi inventario</t>
   </si>
   <si>
@@ -1149,19 +1232,7 @@
 }</t>
   </si>
   <si>
-    <t>Los posibles valores de tipo son:
-1: marco
-2: tijera
-3: ruedas
-4: frenos
-5: manubrio
-6: sillin
-7: tuboSillin
-8: cambios
-9: platoDelantero
-10: platoTrasero
-11: pedales
-12: cadena</t>
+    <t>http://localhost:8080/bicitoolsMi/serviciosRest/miBici/insertarProducto</t>
   </si>
   <si>
     <t>Validar si el usuario que accede al sistema tiene rol de proveedor</t>
@@ -1195,6 +1266,9 @@
     <t>En la respuesta los valores para rol son:
 0: no es proveedor
 1: proveedor</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/bicitoolsMi/serviciosRest/miBici/validarRolProveedor</t>
   </si>
   <si>
     <t>Yo como usuario quiero comprar una parte especifica de una bicicleta</t>
@@ -1223,6 +1297,49 @@
     "valor": "error",
     "descripcion": "Descripción error"
 }</t>
+  </si>
+  <si>
+    <t>Los posibles valores de tipo son:
+1: marco
+2: tijera
+3: ruedas
+4: frenos
+5: manubrio
+6: sillin
+7: cambios
+8: platoDelantero
+9: platoTrasero
+10: pedales
+11: cadena</t>
+  </si>
+  <si>
+    <t>VerOrdenes</t>
+  </si>
+  <si>
+    <t>Yo como usuario quiero ver mis ordenes realizadas </t>
+  </si>
+  <si>
+    <t>{
+   "usuario": "toroj"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "codigo": 0,
+  "valor": "INFO",
+  "descripcion": "OK",
+  "datos": [
+    {
+      "idOrden": "659868",
+      "valor": "645210",
+      "fechaHora": "11/07/2015 16:39:08",
+      "estado": "Pendiente"
+    }
+  ]
+}</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/bicitoolsMi/serviciosRest/miBici/misOrdenes</t>
   </si>
 </sst>
 </file>
@@ -1369,7 +1486,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1389,9 +1506,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1459,9 +1573,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1505,6 +1616,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1810,281 +1942,281 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="3"/>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="236.25">
-      <c r="A2" s="11">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="236.25">
-      <c r="A3" s="11">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="191.25">
-      <c r="A4" s="18">
+      <c r="A4" s="17">
         <v>3</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="I4" s="20" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="135">
-      <c r="A5" s="11">
+      <c r="A5" s="10">
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="16"/>
-      <c r="I5" s="15" t="s">
+      <c r="H5" s="15"/>
+      <c r="I5" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="135">
-      <c r="A6" s="11">
+      <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="16" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="135">
-      <c r="A7" s="11">
+      <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="17" t="s">
+      <c r="H7" s="15"/>
+      <c r="I7" s="16" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="371.25">
-      <c r="A8" s="22">
+      <c r="A8" s="21">
         <v>7</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="26" t="s">
+      <c r="I8" s="25" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="135">
-      <c r="A9" s="11">
+      <c r="A9" s="10">
         <v>8</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="16"/>
-      <c r="I9" s="17" t="s">
+      <c r="H9" s="15"/>
+      <c r="I9" s="16" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="165.75">
-      <c r="A10" s="11">
+      <c r="A10" s="10">
         <v>9</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11" t="s">
+      <c r="H10" s="10"/>
+      <c r="I10" s="10" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2111,246 +2243,246 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" style="30" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" style="29" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="30" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" style="29" customWidth="1"/>
-    <col min="7" max="7" width="78.85546875" style="29" customWidth="1"/>
-    <col min="8" max="8" width="41.7109375" style="30" customWidth="1"/>
-    <col min="9" max="9" width="28.42578125" style="30" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="29" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="28" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="29" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" style="28" customWidth="1"/>
+    <col min="7" max="7" width="78.85546875" style="28" customWidth="1"/>
+    <col min="8" max="8" width="41.7109375" style="29" customWidth="1"/>
+    <col min="9" max="9" width="28.42578125" style="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="29" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="342.75" customHeight="1">
-      <c r="A2" s="28">
+      <c r="A2" s="27">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="I2" s="46" t="s">
+      <c r="I2" s="44" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="342.75" customHeight="1">
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="I3" s="46" t="s">
+      <c r="I3" s="44" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="342.75" customHeight="1">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="I4" s="46" t="s">
+      <c r="I4" s="44" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="306">
-      <c r="A5" s="41">
+      <c r="A5" s="39">
         <v>2</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="43" t="s">
+      <c r="F5" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
     </row>
     <row r="6" spans="1:9" ht="140.25">
-      <c r="A6" s="28">
+      <c r="A6" s="27">
         <v>3</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="I6" s="46" t="s">
+      <c r="I6" s="44" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="45" customFormat="1" ht="204">
-      <c r="A7" s="41">
+    <row r="7" spans="1:9" s="43" customFormat="1" ht="204">
+      <c r="A7" s="39">
         <v>4</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="43" t="s">
+      <c r="F7" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="G7" s="43" t="s">
+      <c r="G7" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="H7" s="44" t="s">
+      <c r="H7" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="I7" s="43"/>
+      <c r="I7" s="41"/>
     </row>
     <row r="8" spans="1:9" ht="139.5" customHeight="1">
-      <c r="A8" s="28">
+      <c r="A8" s="27">
         <v>5</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="G8" s="30"/>
-      <c r="H8" s="40" t="s">
+      <c r="G8" s="29"/>
+      <c r="H8" s="38" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="139.5" customHeight="1">
-      <c r="A9" s="28">
+      <c r="A9" s="27">
         <v>6</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="H9" s="40"/>
+      <c r="H9" s="38"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2373,279 +2505,279 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" style="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" style="33" customWidth="1"/>
-    <col min="3" max="3" width="25" style="33" customWidth="1"/>
-    <col min="4" max="4" width="31" style="33" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="31" customWidth="1"/>
+    <col min="3" max="3" width="25" style="31" customWidth="1"/>
+    <col min="4" max="4" width="31" style="31" customWidth="1"/>
     <col min="5" max="5" width="29.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="27.7109375" customWidth="1"/>
     <col min="7" max="10" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22.5" customHeight="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="30" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="37" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="37" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="37" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="D5" s="39"/>
+      <c r="D5" s="37"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="38" t="s">
+      <c r="B6" s="32"/>
+      <c r="C6" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="37" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="38" t="s">
+      <c r="B7" s="32"/>
+      <c r="C7" s="36" t="s">
         <v>118</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="37" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="38" t="s">
+      <c r="B8" s="32"/>
+      <c r="C8" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="37" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="39" t="s">
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="37" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="35" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="37" t="s">
         <v>127</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="37" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="37" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="D14" s="39" t="s">
+      <c r="D14" s="37" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="D15" s="39" t="s">
+      <c r="D15" s="37" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="34"/>
-      <c r="B16" s="39" t="s">
+      <c r="A16" s="32"/>
+      <c r="B16" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="D16" s="39"/>
+      <c r="D16" s="37"/>
     </row>
     <row r="17" spans="1:4" ht="24">
-      <c r="A17" s="34"/>
-      <c r="B17" s="39" t="s">
+      <c r="A17" s="32"/>
+      <c r="B17" s="37" t="s">
         <v>145</v>
       </c>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="D17" s="34"/>
+      <c r="D17" s="32"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="34"/>
-      <c r="B18" s="39" t="s">
+      <c r="A18" s="32"/>
+      <c r="B18" s="37" t="s">
         <v>147</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="D18" s="34"/>
+      <c r="D18" s="32"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="34"/>
-      <c r="B19" s="39" t="s">
+      <c r="A19" s="32"/>
+      <c r="B19" s="37" t="s">
         <v>149</v>
       </c>
-      <c r="C19" s="39" t="s">
+      <c r="C19" s="37" t="s">
         <v>150</v>
       </c>
-      <c r="D19" s="34"/>
+      <c r="D19" s="32"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="34"/>
-      <c r="B20" s="39" t="s">
+      <c r="A20" s="32"/>
+      <c r="B20" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="C20" s="39" t="s">
+      <c r="C20" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="D20" s="34"/>
+      <c r="D20" s="32"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="34"/>
-      <c r="B21" s="39" t="s">
+      <c r="A21" s="32"/>
+      <c r="B21" s="37" t="s">
         <v>153</v>
       </c>
-      <c r="C21" s="39" t="s">
+      <c r="C21" s="37" t="s">
         <v>154</v>
       </c>
-      <c r="D21" s="34"/>
+      <c r="D21" s="32"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="34"/>
-      <c r="B22" s="39" t="s">
+      <c r="A22" s="32"/>
+      <c r="B22" s="37" t="s">
         <v>155</v>
       </c>
-      <c r="C22" s="39" t="s">
+      <c r="C22" s="37" t="s">
         <v>156</v>
       </c>
-      <c r="D22" s="34"/>
+      <c r="D22" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2654,10 +2786,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -2667,37 +2799,41 @@
     <col min="3" max="3" width="25.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" style="47" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" style="45" customWidth="1"/>
     <col min="7" max="7" width="37.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="45.5703125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="1"/>
+    <col min="8" max="8" width="34.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="3"/>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="225">
+      <c r="I1" s="52" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="45" customFormat="1" ht="213.75">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2705,49 +2841,55 @@
         <v>109</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="236.25">
+        <v>162</v>
+      </c>
+      <c r="I2" s="44" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="409.6">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" ht="315">
+      <c r="I3" s="51" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="45" customFormat="1" ht="315">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -2755,49 +2897,51 @@
         <v>111</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="225">
-      <c r="A5" s="4">
+        <v>174</v>
+      </c>
+      <c r="I4" s="44" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="49" customFormat="1" ht="225">
+      <c r="A5" s="46">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="C5" s="31" t="s">
-        <v>172</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="C5" s="47" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5" s="46" t="s">
+        <v>177</v>
+      </c>
+      <c r="E5" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" ht="135">
+      <c r="F5" s="48" t="s">
+        <v>178</v>
+      </c>
+      <c r="G5" s="48" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="45" customFormat="1" ht="135">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2805,23 +2949,26 @@
         <v>115</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" ht="165.75">
+        <v>183</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="44" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="45" customFormat="1" ht="153">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -2829,25 +2976,28 @@
         <v>116</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="168.75">
+        <v>174</v>
+      </c>
+      <c r="I7" s="44" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="45" customFormat="1" ht="168.75">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -2855,51 +3005,90 @@
         <v>118</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="202.5">
-      <c r="A9" s="4">
+        <v>192</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="I8" s="44" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="49" customFormat="1" ht="202.5">
+      <c r="A9" s="46">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="C9" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="D9" s="46" t="s">
+        <v>177</v>
+      </c>
+      <c r="E9" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="48" t="s">
+        <v>196</v>
+      </c>
+      <c r="G9" s="48" t="s">
+        <v>197</v>
+      </c>
+      <c r="H9" s="46" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="45" customFormat="1" ht="146.25">
+      <c r="A10" s="45">
+        <v>9</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>199</v>
+      </c>
+      <c r="C10" s="45" t="s">
+        <v>200</v>
+      </c>
+      <c r="D10" s="45" t="s">
         <v>190</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>183</v>
+      <c r="E10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="H10" s="29"/>
+      <c r="I10" s="44" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I10" r:id="rId1"/>
+    <hyperlink ref="I2" r:id="rId2"/>
+    <hyperlink ref="I3" r:id="rId3"/>
+    <hyperlink ref="I4" r:id="rId4"/>
+    <hyperlink ref="I6" r:id="rId5"/>
+    <hyperlink ref="I7" r:id="rId6"/>
+    <hyperlink ref="I8" r:id="rId7"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>